<commit_message>
Sprint 2 Acceptance tests
Completed and recorded results for the tests of sprint 2 stories. Most
stories are OK - few are half completed with a bug in the code that
needs fixing. Also updated the sprint plan and burndown charts to
reflect time spent on the tasks
</commit_message>
<xml_diff>
--- a/doc/Burndown Charts/Release 1 Burndown.xlsx
+++ b/doc/Burndown Charts/Release 1 Burndown.xlsx
@@ -711,18 +711,18 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="126148608"/>
-        <c:axId val="126150912"/>
+        <c:axId val="82608512"/>
+        <c:axId val="82610432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126148608"/>
+        <c:axId val="82608512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,14 +798,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126150912"/>
+        <c:crossAx val="82610432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126150912"/>
+        <c:axId val="82610432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -896,7 +896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126148608"/>
+        <c:crossAx val="82608512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -970,7 +970,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1822,7 +1822,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1832,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AC26" sqref="AC26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2356,7 +2356,7 @@
       <c r="U15" s="3">
         <v>1</v>
       </c>
-      <c r="V15" s="2"/>
+      <c r="V15" s="7"/>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="4" t="s">
@@ -2386,7 +2386,7 @@
       <c r="U16" s="3">
         <v>2</v>
       </c>
-      <c r="V16" s="2"/>
+      <c r="V16" s="7"/>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="4" t="s">
@@ -2414,7 +2414,9 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
+      <c r="V17" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="4" t="s">
@@ -2444,7 +2446,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
+      <c r="V18" s="7"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="4" t="s">
@@ -2472,7 +2474,9 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
+      <c r="V19" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="4" t="s">
@@ -2502,7 +2506,7 @@
       <c r="U20" s="3">
         <v>2</v>
       </c>
-      <c r="V20" s="2"/>
+      <c r="V20" s="7"/>
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="4" t="s">
@@ -2532,7 +2536,7 @@
       <c r="U21" s="3">
         <v>1</v>
       </c>
-      <c r="V21" s="2"/>
+      <c r="V21" s="7"/>
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="4" t="s">
@@ -2560,7 +2564,9 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
+      <c r="V22" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="4" t="s">
@@ -2588,7 +2594,7 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
+      <c r="V23" s="7"/>
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="4" t="s">
@@ -2618,7 +2624,7 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
+      <c r="V24" s="7"/>
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="4" t="s">
@@ -2646,7 +2652,7 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
+      <c r="V25" s="7"/>
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="4" t="s">
@@ -2674,7 +2680,9 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
+      <c r="V26" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="4" t="s">
@@ -2704,7 +2712,7 @@
       <c r="U27" s="3">
         <v>0.25</v>
       </c>
-      <c r="V27" s="2"/>
+      <c r="V27" s="7"/>
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="4" t="s">
@@ -2734,7 +2742,7 @@
       <c r="U28" s="3">
         <v>0.25</v>
       </c>
-      <c r="V28" s="2"/>
+      <c r="V28" s="7"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="4" t="s">
@@ -2762,7 +2770,9 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
+      <c r="V29" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="31" spans="1:22" ht="30">
       <c r="A31" s="8" t="s">
@@ -2938,8 +2948,8 @@
         <v>13.5</v>
       </c>
       <c r="V32" s="9">
-        <f t="shared" si="1"/>
-        <v>13.5</v>
+        <f>U32-SUM(V3:V29)-4</f>
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final (??) Sprint progress and burndown charts
</commit_message>
<xml_diff>
--- a/doc/Burndown Charts/Release 1 Burndown.xlsx
+++ b/doc/Burndown Charts/Release 1 Burndown.xlsx
@@ -669,60 +669,60 @@
                   <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.5</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.5</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.5</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.5</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.5</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82608512"/>
-        <c:axId val="82610432"/>
+        <c:axId val="204062080"/>
+        <c:axId val="91031040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82608512"/>
+        <c:axId val="204062080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,14 +798,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82610432"/>
+        <c:crossAx val="91031040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82610432"/>
+        <c:axId val="91031040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -896,7 +896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82608512"/>
+        <c:crossAx val="204062080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -970,7 +970,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1822,7 +1822,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1832,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Z30" sqref="Z30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2168,7 +2168,9 @@
       <c r="E9" s="2"/>
       <c r="F9" s="7"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
       <c r="I9" s="7"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2258,7 +2260,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="13"/>
+      <c r="L12" s="12">
+        <v>0.5</v>
+      </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -2316,7 +2320,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="7"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="13"/>
+      <c r="L14" s="12">
+        <v>0.5</v>
+      </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -2876,7 +2882,7 @@
         <v>34</v>
       </c>
       <c r="D32" s="9">
-        <f t="shared" ref="D32:V32" si="1">C32-SUM(D3:D29)</f>
+        <f t="shared" ref="D32:U32" si="1">C32-SUM(D3:D29)</f>
         <v>33</v>
       </c>
       <c r="E32" s="9">
@@ -2893,63 +2899,63 @@
       </c>
       <c r="H32" s="9">
         <f t="shared" si="1"/>
-        <v>28.5</v>
+        <v>27.5</v>
       </c>
       <c r="I32" s="9">
         <f t="shared" si="1"/>
-        <v>28.5</v>
+        <v>27.5</v>
       </c>
       <c r="J32" s="9">
         <f t="shared" si="1"/>
-        <v>28.5</v>
+        <v>27.5</v>
       </c>
       <c r="K32" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L32" s="9">
         <f t="shared" si="1"/>
-        <v>21.5</v>
+        <v>19.5</v>
       </c>
       <c r="M32" s="9">
         <f t="shared" si="1"/>
-        <v>21.5</v>
+        <v>19.5</v>
       </c>
       <c r="N32" s="9">
         <f t="shared" si="1"/>
-        <v>21.5</v>
+        <v>19.5</v>
       </c>
       <c r="O32" s="9">
         <f t="shared" si="1"/>
-        <v>21.5</v>
+        <v>19.5</v>
       </c>
       <c r="P32" s="9">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q32" s="9">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R32" s="9">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="S32" s="9">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="T32" s="9">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U32" s="9">
         <f t="shared" si="1"/>
-        <v>13.5</v>
+        <v>11.5</v>
       </c>
       <c r="V32" s="9">
-        <f>U32-SUM(V3:V29)-4</f>
-        <v>6.5</v>
+        <f>U32-SUM(V3:V29)-(SUM(B3:B29)-SUM(C3:V29))</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>